<commit_message>
Add [data to books.xlsx]
</commit_message>
<xml_diff>
--- a/Data/books.xlsx
+++ b/Data/books.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Itachi\Documents\GitHub\Library-Management-System\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF53AA9-C7D1-4420-8BA6-E5B187C91350}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718CC859-F87C-4DAD-849E-12E4D97D4CA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="90">
   <si>
     <t>ISBN</t>
   </si>
@@ -156,13 +156,157 @@
   </si>
   <si>
     <t>Frank Herbert</t>
+  </si>
+  <si>
+    <t>Life of Pi</t>
+  </si>
+  <si>
+    <t>Yann Martel</t>
+  </si>
+  <si>
+    <t>The book Thief</t>
+  </si>
+  <si>
+    <t>Markus Zusak</t>
+  </si>
+  <si>
+    <t>Wool</t>
+  </si>
+  <si>
+    <t>Hugh Howey</t>
+  </si>
+  <si>
+    <t>Outlander</t>
+  </si>
+  <si>
+    <t>Diana Gabaldon</t>
+  </si>
+  <si>
+    <t>Wonder</t>
+  </si>
+  <si>
+    <t>R. J. Palacio</t>
+  </si>
+  <si>
+    <t> Ulysses</t>
+  </si>
+  <si>
+    <t>James Joyce</t>
+  </si>
+  <si>
+    <t>Don Quixote</t>
+  </si>
+  <si>
+    <t>Miguel de Cervantes</t>
+  </si>
+  <si>
+    <t>The Great Gatsby</t>
+  </si>
+  <si>
+    <t> F. Scott Fitzgerald</t>
+  </si>
+  <si>
+    <t> One Hundred Years of Solitude</t>
+  </si>
+  <si>
+    <t>Gabriel Garcia Marquez</t>
+  </si>
+  <si>
+    <t>Jurassic Park</t>
+  </si>
+  <si>
+    <t>Michael Chrichton</t>
+  </si>
+  <si>
+    <t>Frankenstein</t>
+  </si>
+  <si>
+    <t> Mary Shelley</t>
+  </si>
+  <si>
+    <t>Foundation</t>
+  </si>
+  <si>
+    <t>Isaac Asimov</t>
+  </si>
+  <si>
+    <t>Solaris</t>
+  </si>
+  <si>
+    <t>Stanislaw Lem</t>
+  </si>
+  <si>
+    <t>When Breath Becomes Air</t>
+  </si>
+  <si>
+    <t>Paul Kalanithi</t>
+  </si>
+  <si>
+    <t>Sapiens: A Brief History of Humankind</t>
+  </si>
+  <si>
+    <t>Yuval Noah Harari</t>
+  </si>
+  <si>
+    <t>Surely You’re Joking, Mr. Feynman!</t>
+  </si>
+  <si>
+    <t>Richard P. Feynman</t>
+  </si>
+  <si>
+    <t>Manual for Living</t>
+  </si>
+  <si>
+    <t>Epictetus</t>
+  </si>
+  <si>
+    <t> CLEAN CODE: A HANDBOOK OF AGILE SOFTWARE CRAFTSMANSHIP</t>
+  </si>
+  <si>
+    <t>Robert C. Martin</t>
+  </si>
+  <si>
+    <t>INTRODUCTION TO ALGORITHMS</t>
+  </si>
+  <si>
+    <t>Thomas H. Cormen</t>
+  </si>
+  <si>
+    <t>WORKING EFFECTIVELY WITH LEGACY CODE</t>
+  </si>
+  <si>
+    <t>Michael Feathers</t>
+  </si>
+  <si>
+    <t>HEAD FIRST JAVA</t>
+  </si>
+  <si>
+    <t>Kathy Sierra</t>
+  </si>
+  <si>
+    <t>A Brief History of Time</t>
+  </si>
+  <si>
+    <t>Stephen Hawking</t>
+  </si>
+  <si>
+    <t> Catch-22</t>
+  </si>
+  <si>
+    <t>Joseph Heller</t>
+  </si>
+  <si>
+    <t>The Illaid</t>
+  </si>
+  <si>
+    <t>Homer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,6 +437,47 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4D5156"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF323232"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF686868"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -639,8 +824,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -996,16 +1192,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.109375" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="56.77734375" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1021,13 +1221,13 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1044,13 +1244,13 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1067,13 +1267,13 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1090,13 +1290,13 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1113,13 +1313,13 @@
       <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1136,13 +1336,13 @@
       <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1159,13 +1359,13 @@
       <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1182,13 +1382,13 @@
       <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1205,13 +1405,13 @@
       <c r="D9" t="s">
         <v>26</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1228,13 +1428,13 @@
       <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1251,13 +1451,13 @@
       <c r="D11" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1274,13 +1474,13 @@
       <c r="D12" t="s">
         <v>26</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>33</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1297,13 +1497,13 @@
       <c r="D13" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1320,13 +1520,13 @@
       <c r="D14" t="s">
         <v>10</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1343,13 +1543,13 @@
       <c r="D15" t="s">
         <v>19</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
         <v>38</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1366,17 +1566,687 @@
       <c r="D16" t="s">
         <v>13</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="4" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>96385274102</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <f ca="1">RANDBETWEEN(1,4)</f>
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>96385274102</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:C41" ca="1" si="0">RANDBETWEEN(1,4)</f>
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f ca="1">RANDBETWEEN(10000000000,99999999999)</f>
+        <v>96641621854</v>
+      </c>
+      <c r="B19">
+        <f>B18+1</f>
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19">
+        <f ca="1">RANDBETWEEN(0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" ref="A20:A41" ca="1" si="1">RANDBETWEEN(10000000000,99999999999)</f>
+        <v>63585113414</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ref="B20:B41" si="2">B19+1</f>
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ref="F20:F41" ca="1" si="3">RANDBETWEEN(0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" ca="1" si="1"/>
+        <v>77451338892</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" ca="1" si="1"/>
+        <v>26759813770</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" ca="1" si="1"/>
+        <v>62711498474</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" ca="1" si="1"/>
+        <v>60261648478</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" ca="1" si="1"/>
+        <v>48304321987</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" ca="1" si="1"/>
+        <v>42616656357</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f t="shared" ca="1" si="1"/>
+        <v>88441408016</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f t="shared" ca="1" si="1"/>
+        <v>55241311913</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" ca="1" si="1"/>
+        <v>30930337099</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" ca="1" si="1"/>
+        <v>83369712399</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F30">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" ca="1" si="1"/>
+        <v>98513825488</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" ca="1" si="1"/>
+        <v>86039057650</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F32">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" ca="1" si="1"/>
+        <v>41370789052</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" ca="1" si="1"/>
+        <v>87598399284</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" ca="1" si="1"/>
+        <v>36695167449</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" ca="1" si="1"/>
+        <v>60438544942</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" ca="1" si="1"/>
+        <v>85802821816</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" ca="1" si="1"/>
+        <v>23095929870</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F38">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <f t="shared" ca="1" si="1"/>
+        <v>15928720190</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F39">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f t="shared" ca="1" si="1"/>
+        <v>85222652019</v>
+      </c>
+      <c r="B40">
+        <f>B39+1</f>
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F40">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f t="shared" ca="1" si="1"/>
+        <v>72425581806</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F41">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>